<commit_message>
changed title names and dash tab layout
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="14400" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Onsite</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Social</t>
   </si>
   <si>
-    <t>Donut values</t>
-  </si>
-  <si>
-    <t>Total campaigns</t>
-  </si>
-  <si>
     <t>Under delivery</t>
   </si>
   <si>
@@ -82,6 +76,63 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>offsite.real</t>
+  </si>
+  <si>
+    <t>onsite.real</t>
+  </si>
+  <si>
+    <t>social.real</t>
+  </si>
+  <si>
+    <t>onsite.donut</t>
+  </si>
+  <si>
+    <t>social.donut</t>
+  </si>
+  <si>
+    <t>underdelivery</t>
+  </si>
+  <si>
+    <t>underdelivery_mom</t>
+  </si>
+  <si>
+    <t>cpc</t>
+  </si>
+  <si>
+    <t>cpc_mom</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>margin_mom</t>
+  </si>
+  <si>
+    <t>ecpm</t>
+  </si>
+  <si>
+    <t>ecpm_mom</t>
+  </si>
+  <si>
+    <t>optimizations</t>
+  </si>
+  <si>
+    <t>optimizations_mom</t>
+  </si>
+  <si>
+    <t>viewability</t>
+  </si>
+  <si>
+    <t>viewability_mom</t>
+  </si>
+  <si>
+    <t>offsite.donut</t>
   </si>
 </sst>
 </file>
@@ -440,7 +491,7 @@
   <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,7 +516,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -477,40 +528,40 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1271,84 +1322,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
-        <f>SUM(B2:D2)</f>
+        <f>SUM(B2+D2+F2)</f>
         <v>4</v>
       </c>
       <c r="B2">
@@ -1356,78 +1419,81 @@
         <v>2</v>
       </c>
       <c r="C2">
+        <f>SUM(100/A2*B2)</f>
+        <v>50</v>
+      </c>
+      <c r="D2">
         <f>SUM(Data!C2:'Data'!C100)</f>
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <f>SUM(100/A2*D2)</f>
+        <v>25</v>
+      </c>
+      <c r="F2">
         <f>SUM(Data!D2:'Data'!D100)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="G2">
+        <f>SUM(100/A2*F2)</f>
+        <v>25</v>
+      </c>
+      <c r="H2" s="4">
         <f>SUM(Data!E2:'Data'!E100)/COUNTA(Data!E2:'Data'!E100)</f>
         <v>4.3200000000000002E-2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="I2" s="3">
         <f>SUM(Data!F2:'Data'!F100)/COUNTA(Data!F2:'Data'!F100)</f>
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="G2" s="5">
+      <c r="J2" s="5">
         <f>SUM(Data!G2:'Data'!G100)/COUNTA(Data!G2:'Data'!G100)</f>
         <v>3.7199999999999998</v>
       </c>
-      <c r="H2" s="3">
+      <c r="K2" s="3">
         <f>SUM(Data!H2:'Data'!H100)/COUNTA(Data!H2:'Data'!H100)</f>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="I2" s="4">
+      <c r="L2" s="4">
         <f>SUM(Data!I2:'Data'!I100)/COUNTA(Data!I2:'Data'!I100)</f>
         <v>0.41849999999999998</v>
       </c>
-      <c r="J2" s="4">
+      <c r="M2" s="4">
         <f>SUM(Data!J2:'Data'!J100)/COUNTA(Data!J2:'Data'!J100)</f>
         <v>0.06</v>
       </c>
-      <c r="K2" s="5">
+      <c r="N2" s="5">
         <f>SUM(Data!K2:'Data'!K100)/COUNTA(Data!K2:'Data'!K100)</f>
         <v>3.69</v>
       </c>
-      <c r="L2" s="4">
+      <c r="O2" s="4">
         <f>SUM(Data!L2:'Data'!L100)/COUNTA(Data!L2:'Data'!L100)</f>
         <v>6.1075000000000004E-2</v>
       </c>
-      <c r="M2" s="6">
+      <c r="P2" s="6">
         <f>SUM(Data!M2:'Data'!M100)/COUNTA(Data!M2:'Data'!M100)</f>
         <v>89</v>
       </c>
-      <c r="N2" s="3">
+      <c r="Q2" s="3">
         <f>SUM(Data!N2:'Data'!N100)/COUNTA(Data!N2:'Data'!N100)</f>
         <v>4.8050000000000002E-2</v>
       </c>
-      <c r="O2" s="4">
+      <c r="R2" s="4">
         <f>SUM(Data!O2:'Data'!O100)/COUNTA(Data!O2:'Data'!O100)</f>
         <v>0.72499999999999998</v>
       </c>
-      <c r="P2" s="3">
+      <c r="S2" s="3">
         <f>SUM(Data!P2:'Data'!P100)/COUNTA(Data!P2:'Data'!P100)</f>
         <v>5.3600000000000009E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <f>SUM(100/A2*B2)</f>
-        <v>50</v>
-      </c>
-      <c r="C4" s="2">
-        <f>SUM(100/A2*C2)</f>
-        <v>25</v>
-      </c>
-      <c r="D4" s="2">
-        <f>SUM(100/A2*D2)</f>
-        <v>25</v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>